<commit_message>
Added Chromedriver, updated excel structure and updated search feature and Stepdefinition
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ClearTripTestData.xlsx
+++ b/src/test/resources/testData/ClearTripTestData.xlsx
@@ -3,19 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Swapnil_Nandurkar\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B94DE1FD-8977-408F-9EBD-677CBCC3CCF0}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B60D8FB7-7675-4F3E-940A-AB95BEBB8906}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4410" xr2:uid="{5F816703-7E63-425E-95E1-41CD349F71CB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13050" windowHeight="5835" xr2:uid="{5F816703-7E63-425E-95E1-41CD349F71CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight_Search" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Chidern</t>
   </si>
@@ -79,16 +75,30 @@
   </si>
   <si>
     <t>TC_0001</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>https://www.cleartrip.com/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -111,14 +121,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81B1C3A-E818-4660-8A1B-C772E4D5C86B}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,10 +458,12 @@
     <col min="5" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="26.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>14</v>
       </c>
@@ -476,8 +491,11 @@
       <c r="I1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -505,8 +523,11 @@
       <c r="I2" s="1">
         <v>2</v>
       </c>
+      <c r="J2" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>15</v>
       </c>
@@ -531,9 +552,15 @@
       <c r="I3" s="1">
         <v>1</v>
       </c>
+      <c r="J3" s="1" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{38BCB6C8-4310-4A75-B011-0A3D4B1CFEF9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Integrated excel utils with steo definition
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ClearTripTestData.xlsx
+++ b/src/test/resources/testData/ClearTripTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{B60D8FB7-7675-4F3E-940A-AB95BEBB8906}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{33329E4E-8946-4FF7-8602-C44132E3C73A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="13050" windowHeight="5835" xr2:uid="{5F816703-7E63-425E-95E1-41CD349F71CB}"/>
   </bookViews>
@@ -16,18 +16,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>Chidern</t>
   </si>
@@ -81,6 +75,15 @@
   </si>
   <si>
     <t>https://www.cleartrip.com/</t>
+  </si>
+  <si>
+    <t>Thu, 14 Feb, 2019</t>
+  </si>
+  <si>
+    <t>Sat, 15 Feb, 2019</t>
+  </si>
+  <si>
+    <t>Thu, 16 Sun, 2019</t>
   </si>
 </sst>
 </file>
@@ -447,7 +450,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,7 +458,8 @@
     <col min="1" max="2" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.140625" style="1"/>
@@ -508,11 +512,11 @@
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="1">
-        <v>43647</v>
-      </c>
-      <c r="F2" s="1">
-        <v>43739</v>
+      <c r="E2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="G2" s="1">
         <v>4</v>
@@ -540,8 +544,8 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1">
-        <v>43647</v>
+      <c r="E3" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="G3" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
Updated code to block notification
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ClearTripTestData.xlsx
+++ b/src/test/resources/testData/ClearTripTestData.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{33329E4E-8946-4FF7-8602-C44132E3C73A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0EFDF2A8-2521-4C5D-BE66-E9FEEFE287F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13050" windowHeight="5835" xr2:uid="{5F816703-7E63-425E-95E1-41CD349F71CB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="5835" xr2:uid="{5F816703-7E63-425E-95E1-41CD349F71CB}"/>
   </bookViews>
   <sheets>
     <sheet name="Flight_Search" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Chidern</t>
   </si>
@@ -77,13 +77,10 @@
     <t>https://www.cleartrip.com/</t>
   </si>
   <si>
-    <t>Thu, 14 Feb, 2019</t>
-  </si>
-  <si>
-    <t>Sat, 15 Feb, 2019</t>
-  </si>
-  <si>
-    <t>Thu, 16 Sun, 2019</t>
+    <t>Wed, 27 Feb, 2019</t>
+  </si>
+  <si>
+    <t>Thu, 28 Feb, 2019</t>
   </si>
 </sst>
 </file>
@@ -450,7 +447,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,7 +542,7 @@
         <v>11</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G3" s="1">
         <v>3</v>

</xml_diff>

<commit_message>
Used DriverManager dependency instead of using chromeDriver.exe
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/ClearTripTestData.xlsx
+++ b/src/test/resources/testData/ClearTripTestData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0EFDF2A8-2521-4C5D-BE66-E9FEEFE287F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{D9910BB1-1116-4D65-9918-7AF3CF76BC95}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15720" windowHeight="5835" xr2:uid="{5F816703-7E63-425E-95E1-41CD349F71CB}"/>
   </bookViews>
@@ -447,7 +447,7 @@
   <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>